<commit_message>
Made some small changes
</commit_message>
<xml_diff>
--- a/bills_input/bills_input.xlsx
+++ b/bills_input/bills_input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Item</t>
   </si>
@@ -22,94 +22,58 @@
     <t>Price</t>
   </si>
   <si>
-    <t xml:space="preserve">700091 EGGS FREE RANGE </t>
-  </si>
-  <si>
     <t xml:space="preserve">45612 MILK WHOLE </t>
   </si>
   <si>
-    <t xml:space="preserve">74032 GARLIC SLICES </t>
-  </si>
-  <si>
-    <t>737083 PLANT MENU TOFU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">700991 POTATOES BAKING </t>
-  </si>
-  <si>
-    <t>812936 SALAD CREAM</t>
-  </si>
-  <si>
-    <t>850426 SQUEEZY MUSTARD</t>
-  </si>
-  <si>
-    <t>52163 MIXED VEG</t>
-  </si>
-  <si>
-    <t>84425 PERI PERI SAUCE</t>
-  </si>
-  <si>
-    <t>727890 SPECIALITY SAUCES</t>
-  </si>
-  <si>
-    <t>741993 CHEESE PANEER</t>
-  </si>
-  <si>
-    <t>731905 CKN DRUM FILLETS</t>
-  </si>
-  <si>
-    <t>700075 EGG NOODLES</t>
-  </si>
-  <si>
-    <t>731223 GRLC BAGUETTE TWIN</t>
-  </si>
-  <si>
     <t>22026 STIR FRY LARGE</t>
   </si>
   <si>
-    <t>828095 SWEET GEM LETTUCE</t>
-  </si>
-  <si>
-    <t>3.10</t>
-  </si>
-  <si>
-    <t>1.09</t>
-  </si>
-  <si>
-    <t>1.78</t>
-  </si>
-  <si>
-    <t>1.58</t>
-  </si>
-  <si>
-    <t>0.89</t>
+    <t>810873 FAMILY PACK TOMATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86247 RICE LG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">727495 TEA GREEN </t>
+  </si>
+  <si>
+    <t>6023 COFFEE DECAF FD</t>
+  </si>
+  <si>
+    <t>836067 PISTACHIOS SALTED</t>
+  </si>
+  <si>
+    <t>42929 BREAD WHOLEMEAL</t>
+  </si>
+  <si>
+    <t>Tortilla</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>2.58</t>
+  </si>
+  <si>
+    <t>1.39</t>
+  </si>
+  <si>
+    <t>1.04</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>0.75</t>
   </si>
   <si>
     <t>0.99</t>
-  </si>
-  <si>
-    <t>1.29</t>
-  </si>
-  <si>
-    <t>0.19</t>
-  </si>
-  <si>
-    <t>1.49</t>
-  </si>
-  <si>
-    <t>2.99</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>2.58</t>
-  </si>
-  <si>
-    <t>1.19</t>
   </si>
 </sst>
 </file>
@@ -467,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -494,7 +458,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -502,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -510,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -518,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -526,7 +490,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -534,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -542,7 +506,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -550,63 +514,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OCR to gradio UI
</commit_message>
<xml_diff>
--- a/bills_input/bills_input.xlsx
+++ b/bills_input/bills_input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -40,15 +40,12 @@
     <t>6023 COFFEE DECAF FD</t>
   </si>
   <si>
-    <t>836067 PISTACHIOS SALTED</t>
+    <t>835067 PISTACHIOS SALTED</t>
   </si>
   <si>
     <t>42929 BREAD WHOLEMEAL</t>
   </si>
   <si>
-    <t>Tortilla</t>
-  </si>
-  <si>
     <t>1.55</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
   </si>
   <si>
     <t>0.75</t>
-  </si>
-  <si>
-    <t>0.99</t>
   </si>
 </sst>
 </file>
@@ -431,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -458,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -466,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -474,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -482,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -490,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -498,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -506,15 +500,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>